<commit_message>
unknown but fixing now
</commit_message>
<xml_diff>
--- a/data/PYPSA_case9_combined.xlsx
+++ b/data/PYPSA_case9_combined.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samho\Desktop\PhD\DC OPF\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393DABEA-C63A-4BDE-A485-4906809AB7F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36009765-0AD5-4FF7-AE4E-2C8D62DC0E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" tabRatio="700" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" tabRatio="700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hvdc" sheetId="12" r:id="rId1"/>
@@ -1270,7 +1270,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F936777E-A678-467D-AA50-B7F1A2F38BF3}">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -5817,8 +5817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T24" sqref="T24"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H111" sqref="H111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>